<commit_message>
update table to include the next poorest model performer
</commit_message>
<xml_diff>
--- a/Overall Models for all production tanks.xlsx
+++ b/Overall Models for all production tanks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Thesis 2023\Capstone---CCT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6CBF0B-E8EA-4CC4-B427-8F0FACE443FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF824618-B7C8-45B4-86B2-2FADE10B1626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{2930D3F1-5665-408B-8E88-0F25E615E518}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{2930D3F1-5665-408B-8E88-0F25E615E518}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="81">
   <si>
     <t>Gradient Boosting Regressor</t>
   </si>
@@ -152,13 +152,160 @@
   </si>
   <si>
     <t xml:space="preserve">Production Batches after Outlier removal </t>
+  </si>
+  <si>
+    <t>Machine Models Performance for each Production Tank Group : All Phases</t>
+  </si>
+  <si>
+    <t>Simple Neural Network</t>
+  </si>
+  <si>
+    <t>Support Vector Machine</t>
+  </si>
+  <si>
+    <t>K-Nearest Neighbors</t>
+  </si>
+  <si>
+    <r>
+      <t>K-Nearest Neighbors (After Tuning)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF374151"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <t>Machine Model and Results  for Production Tanks  25MT 10  Gum Addition Phases</t>
+  </si>
+  <si>
+    <t>Model Type</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Train MSE</t>
+  </si>
+  <si>
+    <t>Train MSE- Tuned</t>
+  </si>
+  <si>
+    <t>Test MSE</t>
+  </si>
+  <si>
+    <t>Test MSE- Tuned</t>
+  </si>
+  <si>
+    <t>Train R2</t>
+  </si>
+  <si>
+    <t>Train R2- Tuned</t>
+  </si>
+  <si>
+    <t>Test R2</t>
+  </si>
+  <si>
+    <t>Test R2- Tuned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Best Parameters </t>
+  </si>
+  <si>
+    <t>Linear</t>
+  </si>
+  <si>
+    <t>Linear Regression</t>
+  </si>
+  <si>
+    <t>Ridge Regression</t>
+  </si>
+  <si>
+    <t>alpha': 0.01</t>
+  </si>
+  <si>
+    <t>Lasso Regression</t>
+  </si>
+  <si>
+    <t>Ensemble/Tree Based</t>
+  </si>
+  <si>
+    <t>Random Forest Regressor</t>
+  </si>
+  <si>
+    <t>max_depth': 20, 'n_estimators': 200</t>
+  </si>
+  <si>
+    <t>learning_rate': 0.2, 'max_depth': 3, 'n_estimators': 100</t>
+  </si>
+  <si>
+    <t>Tree Based</t>
+  </si>
+  <si>
+    <t>Decision Tree Regressor</t>
+  </si>
+  <si>
+    <t>max_depth': 10</t>
+  </si>
+  <si>
+    <t>Ensemble</t>
+  </si>
+  <si>
+    <t>Bagging Regressor</t>
+  </si>
+  <si>
+    <t>max_features': 1.0, 'max_samples': 1.0, 'n_estimators': 200</t>
+  </si>
+  <si>
+    <t>Instance based</t>
+  </si>
+  <si>
+    <t>Fitting 5 folds for each of 32 candidates, totalling 160 fits
+algorithm': 'auto', 'n_neighbors': 5, 'weights': 'distance'</t>
+  </si>
+  <si>
+    <t>Kernal Based</t>
+  </si>
+  <si>
+    <t>Fitting 5 folds for each of 36 candidates, totalling 180 fits
+'C': 1, 'degree': 2, 'gamma': 'scale', 'kernel': 'linear'</t>
+  </si>
+  <si>
+    <t>Neural Network ( FCN)</t>
+  </si>
+  <si>
+    <t>Dense Neural Network</t>
+  </si>
+  <si>
+    <t>neurons_layer3': 16, 'neurons_layer2': 128, 'neurons_layer1': 64, 'epochs': 50, 'batch_size': 16</t>
+  </si>
+  <si>
+    <t>Neural Network</t>
+  </si>
+  <si>
+    <t>neurons_layer2': 32, 'neurons_layer1': 128, 'epochs': 50, 'batch_size': 32
+Fitting 3 folds for each of 5 candidates, totalling 15 fits</t>
+  </si>
+  <si>
+    <t>Neural Network ( RNN)</t>
+  </si>
+  <si>
+    <t>LSTM Neural Network</t>
+  </si>
+  <si>
+    <t>lstm_neurons': 30, 'epochs': 50, 'batch_size': 16
+import pandas as pd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,8 +354,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF374151"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,8 +393,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -288,11 +466,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -338,6 +553,72 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1011,10 +1292,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E644C826-A6FB-44B9-865C-DA5DDDDA09A0}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,11 +1304,12 @@
     <col min="4" max="4" width="19.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="25" style="2" customWidth="1"/>
     <col min="6" max="6" width="26.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -1035,7 +1317,7 @@
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -1055,7 +1337,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1074,8 +1356,11 @@
       <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -1094,8 +1379,9 @@
       <c r="F4" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>19</v>
       </c>
@@ -1114,8 +1400,11 @@
       <c r="F5" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>20</v>
       </c>
@@ -1134,8 +1423,11 @@
       <c r="F6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
@@ -1154,6 +1446,7 @@
       <c r="F7" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G7" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1165,22 +1458,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F4CDC16-0C58-41B3-B49C-552739BFDEB4}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="3" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" customWidth="1"/>
     <col min="5" max="5" width="26.28515625" customWidth="1"/>
     <col min="6" max="6" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>25</v>
       </c>
@@ -1190,7 +1484,7 @@
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -1210,7 +1504,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1229,8 +1523,11 @@
       <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -1250,7 +1547,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>19</v>
       </c>
@@ -1269,8 +1566,11 @@
       <c r="F5" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>20</v>
       </c>
@@ -1289,8 +1589,11 @@
       <c r="F6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
@@ -1323,7 +1626,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,14 +1639,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -1475,10 +1778,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{511F3F11-9483-4742-8A44-7B6D16CBE82D}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6:Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1490,7 +1793,7 @@
     <col min="6" max="6" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>25</v>
       </c>
@@ -1500,7 +1803,7 @@
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -1520,7 +1823,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1540,7 +1843,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -1560,7 +1863,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>19</v>
       </c>
@@ -1579,8 +1882,11 @@
       <c r="F5" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>20</v>
       </c>
@@ -1599,8 +1905,21 @@
       <c r="F6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="24"/>
+      <c r="H6" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
+    </row>
+    <row r="7" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
@@ -1619,10 +1938,456 @@
       <c r="F7" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G7" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="L7" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="M7" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="O7" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="P7" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q7" s="27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G8" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="30">
+        <v>3.6443660425788862E-3</v>
+      </c>
+      <c r="J8" s="31">
+        <v>3.6443660425788862E-3</v>
+      </c>
+      <c r="K8" s="30">
+        <v>1.7224902754740239E-3</v>
+      </c>
+      <c r="L8" s="31">
+        <v>1.7224902754740239E-3</v>
+      </c>
+      <c r="M8" s="30">
+        <v>0.9959288874309985</v>
+      </c>
+      <c r="N8" s="31">
+        <v>0.9959288874309985</v>
+      </c>
+      <c r="O8" s="30">
+        <v>0.99846139886603147</v>
+      </c>
+      <c r="P8" s="31">
+        <v>0.99846139886603147</v>
+      </c>
+      <c r="Q8" s="32"/>
+    </row>
+    <row r="9" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="G9" s="33"/>
+      <c r="H9" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" s="30">
+        <v>4.2117159990730704E-3</v>
+      </c>
+      <c r="J9" s="31">
+        <v>3.6507038277135899E-3</v>
+      </c>
+      <c r="K9" s="30">
+        <v>3.2802679545766572E-3</v>
+      </c>
+      <c r="L9" s="31">
+        <v>1.8093407576561091E-3</v>
+      </c>
+      <c r="M9" s="30">
+        <v>0.99529510215478856</v>
+      </c>
+      <c r="N9" s="31">
+        <v>0.99592180750641901</v>
+      </c>
+      <c r="O9" s="30">
+        <v>0.99706992598652366</v>
+      </c>
+      <c r="P9" s="31">
+        <v>0.99838382034365969</v>
+      </c>
+      <c r="Q9" s="32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="G10" s="34"/>
+      <c r="H10" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="30">
+        <v>0.7808632570284062</v>
+      </c>
+      <c r="J10" s="31">
+        <v>3.8056440707204871E-3</v>
+      </c>
+      <c r="K10" s="30">
+        <v>1.112008925877159</v>
+      </c>
+      <c r="L10" s="31">
+        <v>2.4247514985234839E-3</v>
+      </c>
+      <c r="M10" s="30">
+        <v>0.12769952764945991</v>
+      </c>
+      <c r="N10" s="31">
+        <v>0.99574872413241655</v>
+      </c>
+      <c r="O10" s="30">
+        <v>6.7066161712646677E-3</v>
+      </c>
+      <c r="P10" s="31">
+        <v>0.99783410945284245</v>
+      </c>
+      <c r="Q10" s="35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="51" x14ac:dyDescent="0.25">
+      <c r="G11" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="30">
+        <v>2.6684229494021139E-3</v>
+      </c>
+      <c r="J11" s="31">
+        <v>3.2712767751849649E-3</v>
+      </c>
+      <c r="K11" s="30">
+        <v>1.6113729686535232E-2</v>
+      </c>
+      <c r="L11" s="31">
+        <v>1.498281247503907E-2</v>
+      </c>
+      <c r="M11" s="30">
+        <v>0.99701911112061736</v>
+      </c>
+      <c r="N11" s="31">
+        <v>0.99634566455714357</v>
+      </c>
+      <c r="O11" s="30">
+        <v>0.9856065354207344</v>
+      </c>
+      <c r="P11" s="31">
+        <v>0.98661671848464372</v>
+      </c>
+      <c r="Q11" s="35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="G12" s="34"/>
+      <c r="H12" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="30">
+        <v>4.4416365163711717E-5</v>
+      </c>
+      <c r="J12" s="31">
+        <v>2.2573613228534591E-11</v>
+      </c>
+      <c r="K12" s="30">
+        <v>9.7202296156545243E-3</v>
+      </c>
+      <c r="L12" s="31">
+        <v>9.5781780831869293E-3</v>
+      </c>
+      <c r="M12" s="30">
+        <v>0.99995038258496138</v>
+      </c>
+      <c r="N12" s="31">
+        <v>0.99999999997478306</v>
+      </c>
+      <c r="O12" s="30">
+        <v>0.99131747997534303</v>
+      </c>
+      <c r="P12" s="31">
+        <v>0.99144436640950673</v>
+      </c>
+      <c r="Q12" s="35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="G13" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="I13" s="30">
+        <v>0</v>
+      </c>
+      <c r="J13" s="31">
+        <v>0</v>
+      </c>
+      <c r="K13" s="30">
+        <v>1.679357553792437E-2</v>
+      </c>
+      <c r="L13" s="31">
+        <v>1.8256332536202541E-2</v>
+      </c>
+      <c r="M13" s="30">
+        <v>1</v>
+      </c>
+      <c r="N13" s="31">
+        <v>1</v>
+      </c>
+      <c r="O13" s="30">
+        <v>0.9849992683651434</v>
+      </c>
+      <c r="P13" s="31">
+        <v>0.98369267197483767</v>
+      </c>
+      <c r="Q13" s="32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="G14" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="I14" s="30">
+        <v>3.43300276888928E-3</v>
+      </c>
+      <c r="J14" s="31">
+        <v>4.1647866029152899E-3</v>
+      </c>
+      <c r="K14" s="30">
+        <v>1.7474633086577009E-2</v>
+      </c>
+      <c r="L14" s="31">
+        <v>1.9727261282711499E-2</v>
+      </c>
+      <c r="M14" s="30">
+        <v>0.99616500083730553</v>
+      </c>
+      <c r="N14" s="31">
+        <v>0.99534752687072581</v>
+      </c>
+      <c r="O14" s="30">
+        <v>0.98439091897033115</v>
+      </c>
+      <c r="P14" s="31">
+        <v>0.98237877623354375</v>
+      </c>
+      <c r="Q14" s="32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="153" x14ac:dyDescent="0.25">
+      <c r="G15" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" s="30">
+        <v>583.72199999999998</v>
+      </c>
+      <c r="J15" s="31">
+        <v>0</v>
+      </c>
+      <c r="K15" s="30">
+        <v>1477.1</v>
+      </c>
+      <c r="L15" s="31">
+        <v>1</v>
+      </c>
+      <c r="M15" s="30">
+        <v>0.92204299999999995</v>
+      </c>
+      <c r="N15" s="31">
+        <v>0.92204299999999995</v>
+      </c>
+      <c r="O15" s="30">
+        <v>0.84226199999999996</v>
+      </c>
+      <c r="P15" s="31">
+        <v>0.82208800000000004</v>
+      </c>
+      <c r="Q15" s="37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="153" x14ac:dyDescent="0.25">
+      <c r="G16" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="H16" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="I16" s="30">
+        <v>7398.89</v>
+      </c>
+      <c r="J16" s="31">
+        <v>34.7301</v>
+      </c>
+      <c r="K16" s="30">
+        <v>15081.1</v>
+      </c>
+      <c r="L16" s="31">
+        <v>0.99536199999999997</v>
+      </c>
+      <c r="M16" s="30">
+        <v>1.18674E-2</v>
+      </c>
+      <c r="N16" s="31">
+        <v>1.18674E-2</v>
+      </c>
+      <c r="O16" s="30">
+        <v>-0.61049799999999999</v>
+      </c>
+      <c r="P16" s="31">
+        <v>0.99725900000000001</v>
+      </c>
+      <c r="Q16" s="37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="7:17" ht="140.25" x14ac:dyDescent="0.25">
+      <c r="G17" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="H17" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="I17" s="30">
+        <v>1016.37</v>
+      </c>
+      <c r="J17" s="31">
+        <v>169.435</v>
+      </c>
+      <c r="K17" s="30">
+        <v>994.49900000000002</v>
+      </c>
+      <c r="L17" s="31">
+        <v>213.714</v>
+      </c>
+      <c r="M17" s="30">
+        <v>0.86426199999999997</v>
+      </c>
+      <c r="N17" s="31">
+        <v>0.97737200000000002</v>
+      </c>
+      <c r="O17" s="30">
+        <v>0.89379799999999998</v>
+      </c>
+      <c r="P17" s="31">
+        <v>0.97717799999999999</v>
+      </c>
+      <c r="Q17" s="35" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="7:17" ht="191.25" x14ac:dyDescent="0.25">
+      <c r="G18" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="30">
+        <v>15748.4</v>
+      </c>
+      <c r="J18" s="31">
+        <v>378.85156545293802</v>
+      </c>
+      <c r="K18" s="30">
+        <v>29627.200000000001</v>
+      </c>
+      <c r="L18" s="31">
+        <v>491.046564278326</v>
+      </c>
+      <c r="M18" s="30">
+        <v>-1.1032200000000001</v>
+      </c>
+      <c r="N18" s="31">
+        <v>0.94940379111289996</v>
+      </c>
+      <c r="O18" s="30">
+        <v>-2.1638600000000001</v>
+      </c>
+      <c r="P18" s="31">
+        <v>0.94756156556688498</v>
+      </c>
+      <c r="Q18" s="35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="7:17" ht="115.5" x14ac:dyDescent="0.25">
+      <c r="G19" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="I19" s="30">
+        <v>18366.099999999999</v>
+      </c>
+      <c r="J19" s="31">
+        <v>11195.507941412599</v>
+      </c>
+      <c r="K19" s="30">
+        <v>34292.400000000001</v>
+      </c>
+      <c r="L19" s="31">
+        <v>20525.288342845299</v>
+      </c>
+      <c r="M19" s="30">
+        <v>-1.45282</v>
+      </c>
+      <c r="N19" s="31">
+        <v>-0.49517729383979597</v>
+      </c>
+      <c r="O19" s="30">
+        <v>-2.6620599999999999</v>
+      </c>
+      <c r="P19" s="31">
+        <v>-1.19187764518602</v>
+      </c>
+      <c r="Q19" s="39" t="s">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H6:Q6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1632,8 +2397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DC71460-FAB3-4070-807A-7EE168D0F0F4}">
   <dimension ref="A2:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated and reviewed results
</commit_message>
<xml_diff>
--- a/Overall Models for all production tanks.xlsx
+++ b/Overall Models for all production tanks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Thesis 2023\Capstone---CCT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF824618-B7C8-45B4-86B2-2FADE10B1626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD635AA2-0C18-4684-BF35-F93D942FD9FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{2930D3F1-5665-408B-8E88-0F25E615E518}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{2930D3F1-5665-408B-8E88-0F25E615E518}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Agitation" sheetId="4" r:id="rId4"/>
     <sheet name="Gum Addition " sheetId="5" r:id="rId5"/>
     <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="84">
   <si>
     <t>Gradient Boosting Regressor</t>
   </si>
@@ -180,132 +181,137 @@
     </r>
   </si>
   <si>
-    <t>Machine Model and Results  for Production Tanks  25MT 10  Gum Addition Phases</t>
-  </si>
-  <si>
-    <t>Model Type</t>
-  </si>
-  <si>
     <t>Model</t>
   </si>
   <si>
-    <t>Train MSE</t>
-  </si>
-  <si>
-    <t>Train MSE- Tuned</t>
-  </si>
-  <si>
-    <t>Test MSE</t>
-  </si>
-  <si>
-    <t>Test MSE- Tuned</t>
-  </si>
-  <si>
-    <t>Train R2</t>
-  </si>
-  <si>
-    <t>Train R2- Tuned</t>
-  </si>
-  <si>
-    <t>Test R2</t>
-  </si>
-  <si>
-    <t>Test R2- Tuned</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Best Parameters </t>
-  </si>
-  <si>
-    <t>Linear</t>
-  </si>
-  <si>
     <t>Linear Regression</t>
   </si>
   <si>
     <t>Ridge Regression</t>
   </si>
   <si>
-    <t>alpha': 0.01</t>
-  </si>
-  <si>
     <t>Lasso Regression</t>
   </si>
   <si>
-    <t>Ensemble/Tree Based</t>
-  </si>
-  <si>
     <t>Random Forest Regressor</t>
   </si>
   <si>
-    <t>max_depth': 20, 'n_estimators': 200</t>
-  </si>
-  <si>
-    <t>learning_rate': 0.2, 'max_depth': 3, 'n_estimators': 100</t>
-  </si>
-  <si>
-    <t>Tree Based</t>
-  </si>
-  <si>
     <t>Decision Tree Regressor</t>
   </si>
   <si>
-    <t>max_depth': 10</t>
-  </si>
-  <si>
-    <t>Ensemble</t>
-  </si>
-  <si>
     <t>Bagging Regressor</t>
   </si>
   <si>
-    <t>max_features': 1.0, 'max_samples': 1.0, 'n_estimators': 200</t>
-  </si>
-  <si>
-    <t>Instance based</t>
-  </si>
-  <si>
-    <t>Fitting 5 folds for each of 32 candidates, totalling 160 fits
-algorithm': 'auto', 'n_neighbors': 5, 'weights': 'distance'</t>
-  </si>
-  <si>
-    <t>Kernal Based</t>
-  </si>
-  <si>
-    <t>Fitting 5 folds for each of 36 candidates, totalling 180 fits
-'C': 1, 'degree': 2, 'gamma': 'scale', 'kernel': 'linear'</t>
-  </si>
-  <si>
-    <t>Neural Network ( FCN)</t>
-  </si>
-  <si>
-    <t>Dense Neural Network</t>
-  </si>
-  <si>
-    <t>neurons_layer3': 16, 'neurons_layer2': 128, 'neurons_layer1': 64, 'epochs': 50, 'batch_size': 16</t>
-  </si>
-  <si>
-    <t>Neural Network</t>
-  </si>
-  <si>
-    <t>neurons_layer2': 32, 'neurons_layer1': 128, 'epochs': 50, 'batch_size': 32
-Fitting 3 folds for each of 5 candidates, totalling 15 fits</t>
-  </si>
-  <si>
-    <t>Neural Network ( RNN)</t>
-  </si>
-  <si>
-    <t>LSTM Neural Network</t>
-  </si>
-  <si>
-    <t>lstm_neurons': 30, 'epochs': 50, 'batch_size': 16
-import pandas as pd</t>
+    <t>Hyperparameters</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>No hyperparameters are tuned since it's a straightforward algorithm.</t>
+  </si>
+  <si>
+    <t>alpha: [0.01, 0.1, 1.0, 10.0]</t>
+  </si>
+  <si>
+    <t>A common range for the regularization parameter, covering a spectrum from light to strong regularization.</t>
+  </si>
+  <si>
+    <t>Similar to Ridge, this is a common range for regularization intensity.</t>
+  </si>
+  <si>
+    <t>max_depth: [None, 10, 20]</t>
+  </si>
+  <si>
+    <t>Offers a choice between a shallow tree, a deeper tree, and a fully grown tree.</t>
+  </si>
+  <si>
+    <t>Provides variability in base estimators and how much of the dataset and features they should consider.</t>
+  </si>
+  <si>
+    <t>AdaBoost Regressor</t>
+  </si>
+  <si>
+    <t>Covers various configurations of neighbors and algorithms to account for dataset's characteristics.</t>
+  </si>
+  <si>
+    <t>Simple Neural Network (Keras)</t>
+  </si>
+  <si>
+    <t>Covers various neuron counts for two dense layers and different training strategies.</t>
+  </si>
+  <si>
+    <t>LSTM (Keras)</t>
+  </si>
+  <si>
+    <t>Tuning for LSTM models can be computationally intensive. This setup offers flexibility in LSTM neuron counts and training parameters.</t>
+  </si>
+  <si>
+    <t>Simple Dense Neural Network</t>
+  </si>
+  <si>
+    <t>A basic three-layer feedforward neural network.</t>
+  </si>
+  <si>
+    <t>Dense Neural Network (Optimized via RandomizedSearchCV)</t>
+  </si>
+  <si>
+    <t>Random grid search over different configurations, sampling 10 combinations. The goal is to find an optimal architecture and training configuration for the neural network.</t>
+  </si>
+  <si>
+    <t>Layers: [128, 64, 32], epochs: 50, batch_size: 32</t>
+  </si>
+  <si>
+    <t>batch_size: [16, 32, 64], epochs: [20, 50, 100], neurons_layer1: [64, 128, 256], neurons_layer2: [32, 64, 128], neurons_layer3: [16, 32, 64]</t>
+  </si>
+  <si>
+    <t>n_estimators: [100, 200, 300], max_depth: [None, 10, 20]</t>
+  </si>
+  <si>
+    <t>A reasonable starting range. Consider testing more n_estimators based on computational constraints.</t>
+  </si>
+  <si>
+    <t>n_estimators: [100, 200, 300], learning_rate: [0.01, 0.1, 0.2], max_depth: [3, 4, 5]</t>
+  </si>
+  <si>
+    <t>The interplay between learning_rate and n_estimators is important. Depending on resources, a broader range for n_estimators might be considered.</t>
+  </si>
+  <si>
+    <t>n_estimators: [50, 100, 200], max_samples: [0.5, 0.7, 1.0], max_features: [0.5, 0.7, 1.0]</t>
+  </si>
+  <si>
+    <t>n_estimators: [50, 100, 200], learning_rate: [0.01, 0.05, 0.1]</t>
+  </si>
+  <si>
+    <t>Interplay between learning_rate and n_estimators is key. Values can be quite dataset-specific.</t>
+  </si>
+  <si>
+    <t>n_neighbors: [3, 5, 7, 9], weights: ['uniform', 'distance'], algorithm: ['auto', 'ball_tree', 'kd_tree', 'brute']</t>
+  </si>
+  <si>
+    <t>C: [0.1, 1, 10], kernel: ['rbf', 'linear', 'poly'], degree: [2, 3], gamma: ['scale', 'auto']</t>
+  </si>
+  <si>
+    <t>Incorporates various kernel functions and regularization strengths. Note that some combinations might not be meaningful (e.g., degree with rbf).</t>
+  </si>
+  <si>
+    <t>dense1_neurons: [32, 64, 128], dense2_neurons: [16, 32, 64], epochs: [30, 50], batch_size: [16, 32, 64]</t>
+  </si>
+  <si>
+    <t>lstm_neurons: [30, 50, 70], batch_size: [16, 32, 64], epochs: [30, 50, 100]</t>
+  </si>
+  <si>
+    <t>Breakdown per Machine Learning Model for Hyperparameter Tuning</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -367,14 +373,19 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF374151"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF374151"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -393,20 +404,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -490,24 +489,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -569,56 +555,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -936,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33222403-0FAA-476C-9669-B9B11CFC086D}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection sqref="A1:E26"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,7 +1245,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1427,7 +1377,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
@@ -1446,7 +1396,9 @@
       <c r="F7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="21"/>
+      <c r="G7" s="19" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1461,7 +1413,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1523,7 +1475,7 @@
       <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="22" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1593,7 +1545,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
@@ -1611,6 +1563,9 @@
       </c>
       <c r="F7" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1626,7 +1581,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1778,10 +1733,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{511F3F11-9483-4742-8A44-7B6D16CBE82D}">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:Q19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1793,7 +1748,7 @@
     <col min="6" max="6" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>25</v>
       </c>
@@ -1803,7 +1758,7 @@
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -1823,7 +1778,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1843,7 +1798,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -1863,7 +1818,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>19</v>
       </c>
@@ -1886,7 +1841,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>20</v>
       </c>
@@ -1905,21 +1860,11 @@
       <c r="F6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26"/>
-    </row>
-    <row r="7" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="G6" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
@@ -1938,456 +1883,10 @@
       <c r="F7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="J7" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="K7" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="L7" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="M7" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="N7" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="O7" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="P7" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q7" s="27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G8" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="H8" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="I8" s="30">
-        <v>3.6443660425788862E-3</v>
-      </c>
-      <c r="J8" s="31">
-        <v>3.6443660425788862E-3</v>
-      </c>
-      <c r="K8" s="30">
-        <v>1.7224902754740239E-3</v>
-      </c>
-      <c r="L8" s="31">
-        <v>1.7224902754740239E-3</v>
-      </c>
-      <c r="M8" s="30">
-        <v>0.9959288874309985</v>
-      </c>
-      <c r="N8" s="31">
-        <v>0.9959288874309985</v>
-      </c>
-      <c r="O8" s="30">
-        <v>0.99846139886603147</v>
-      </c>
-      <c r="P8" s="31">
-        <v>0.99846139886603147</v>
-      </c>
-      <c r="Q8" s="32"/>
-    </row>
-    <row r="9" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="G9" s="33"/>
-      <c r="H9" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="I9" s="30">
-        <v>4.2117159990730704E-3</v>
-      </c>
-      <c r="J9" s="31">
-        <v>3.6507038277135899E-3</v>
-      </c>
-      <c r="K9" s="30">
-        <v>3.2802679545766572E-3</v>
-      </c>
-      <c r="L9" s="31">
-        <v>1.8093407576561091E-3</v>
-      </c>
-      <c r="M9" s="30">
-        <v>0.99529510215478856</v>
-      </c>
-      <c r="N9" s="31">
-        <v>0.99592180750641901</v>
-      </c>
-      <c r="O9" s="30">
-        <v>0.99706992598652366</v>
-      </c>
-      <c r="P9" s="31">
-        <v>0.99838382034365969</v>
-      </c>
-      <c r="Q9" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="G10" s="34"/>
-      <c r="H10" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10" s="30">
-        <v>0.7808632570284062</v>
-      </c>
-      <c r="J10" s="31">
-        <v>3.8056440707204871E-3</v>
-      </c>
-      <c r="K10" s="30">
-        <v>1.112008925877159</v>
-      </c>
-      <c r="L10" s="31">
-        <v>2.4247514985234839E-3</v>
-      </c>
-      <c r="M10" s="30">
-        <v>0.12769952764945991</v>
-      </c>
-      <c r="N10" s="31">
-        <v>0.99574872413241655</v>
-      </c>
-      <c r="O10" s="30">
-        <v>6.7066161712646677E-3</v>
-      </c>
-      <c r="P10" s="31">
-        <v>0.99783410945284245</v>
-      </c>
-      <c r="Q10" s="35" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="G11" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="H11" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="I11" s="30">
-        <v>2.6684229494021139E-3</v>
-      </c>
-      <c r="J11" s="31">
-        <v>3.2712767751849649E-3</v>
-      </c>
-      <c r="K11" s="30">
-        <v>1.6113729686535232E-2</v>
-      </c>
-      <c r="L11" s="31">
-        <v>1.498281247503907E-2</v>
-      </c>
-      <c r="M11" s="30">
-        <v>0.99701911112061736</v>
-      </c>
-      <c r="N11" s="31">
-        <v>0.99634566455714357</v>
-      </c>
-      <c r="O11" s="30">
-        <v>0.9856065354207344</v>
-      </c>
-      <c r="P11" s="31">
-        <v>0.98661671848464372</v>
-      </c>
-      <c r="Q11" s="35" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="G12" s="34"/>
-      <c r="H12" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="I12" s="30">
-        <v>4.4416365163711717E-5</v>
-      </c>
-      <c r="J12" s="31">
-        <v>2.2573613228534591E-11</v>
-      </c>
-      <c r="K12" s="30">
-        <v>9.7202296156545243E-3</v>
-      </c>
-      <c r="L12" s="31">
-        <v>9.5781780831869293E-3</v>
-      </c>
-      <c r="M12" s="30">
-        <v>0.99995038258496138</v>
-      </c>
-      <c r="N12" s="31">
-        <v>0.99999999997478306</v>
-      </c>
-      <c r="O12" s="30">
-        <v>0.99131747997534303</v>
-      </c>
-      <c r="P12" s="31">
-        <v>0.99144436640950673</v>
-      </c>
-      <c r="Q12" s="35" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="G13" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="H13" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="I13" s="30">
-        <v>0</v>
-      </c>
-      <c r="J13" s="31">
-        <v>0</v>
-      </c>
-      <c r="K13" s="30">
-        <v>1.679357553792437E-2</v>
-      </c>
-      <c r="L13" s="31">
-        <v>1.8256332536202541E-2</v>
-      </c>
-      <c r="M13" s="30">
-        <v>1</v>
-      </c>
-      <c r="N13" s="31">
-        <v>1</v>
-      </c>
-      <c r="O13" s="30">
-        <v>0.9849992683651434</v>
-      </c>
-      <c r="P13" s="31">
-        <v>0.98369267197483767</v>
-      </c>
-      <c r="Q13" s="32" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="G14" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="H14" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="I14" s="30">
-        <v>3.43300276888928E-3</v>
-      </c>
-      <c r="J14" s="31">
-        <v>4.1647866029152899E-3</v>
-      </c>
-      <c r="K14" s="30">
-        <v>1.7474633086577009E-2</v>
-      </c>
-      <c r="L14" s="31">
-        <v>1.9727261282711499E-2</v>
-      </c>
-      <c r="M14" s="30">
-        <v>0.99616500083730553</v>
-      </c>
-      <c r="N14" s="31">
-        <v>0.99534752687072581</v>
-      </c>
-      <c r="O14" s="30">
-        <v>0.98439091897033115</v>
-      </c>
-      <c r="P14" s="31">
-        <v>0.98237877623354375</v>
-      </c>
-      <c r="Q14" s="32" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="153" x14ac:dyDescent="0.25">
-      <c r="G15" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="I15" s="30">
-        <v>583.72199999999998</v>
-      </c>
-      <c r="J15" s="31">
-        <v>0</v>
-      </c>
-      <c r="K15" s="30">
-        <v>1477.1</v>
-      </c>
-      <c r="L15" s="31">
-        <v>1</v>
-      </c>
-      <c r="M15" s="30">
-        <v>0.92204299999999995</v>
-      </c>
-      <c r="N15" s="31">
-        <v>0.92204299999999995</v>
-      </c>
-      <c r="O15" s="30">
-        <v>0.84226199999999996</v>
-      </c>
-      <c r="P15" s="31">
-        <v>0.82208800000000004</v>
-      </c>
-      <c r="Q15" s="37" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="153" x14ac:dyDescent="0.25">
-      <c r="G16" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="H16" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="I16" s="30">
-        <v>7398.89</v>
-      </c>
-      <c r="J16" s="31">
-        <v>34.7301</v>
-      </c>
-      <c r="K16" s="30">
-        <v>15081.1</v>
-      </c>
-      <c r="L16" s="31">
-        <v>0.99536199999999997</v>
-      </c>
-      <c r="M16" s="30">
-        <v>1.18674E-2</v>
-      </c>
-      <c r="N16" s="31">
-        <v>1.18674E-2</v>
-      </c>
-      <c r="O16" s="30">
-        <v>-0.61049799999999999</v>
-      </c>
-      <c r="P16" s="31">
-        <v>0.99725900000000001</v>
-      </c>
-      <c r="Q16" s="37" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="7:17" ht="140.25" x14ac:dyDescent="0.25">
-      <c r="G17" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="H17" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="I17" s="30">
-        <v>1016.37</v>
-      </c>
-      <c r="J17" s="31">
-        <v>169.435</v>
-      </c>
-      <c r="K17" s="30">
-        <v>994.49900000000002</v>
-      </c>
-      <c r="L17" s="31">
-        <v>213.714</v>
-      </c>
-      <c r="M17" s="30">
-        <v>0.86426199999999997</v>
-      </c>
-      <c r="N17" s="31">
-        <v>0.97737200000000002</v>
-      </c>
-      <c r="O17" s="30">
-        <v>0.89379799999999998</v>
-      </c>
-      <c r="P17" s="31">
-        <v>0.97717799999999999</v>
-      </c>
-      <c r="Q17" s="35" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="7:17" ht="191.25" x14ac:dyDescent="0.25">
-      <c r="G18" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="H18" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="I18" s="30">
-        <v>15748.4</v>
-      </c>
-      <c r="J18" s="31">
-        <v>378.85156545293802</v>
-      </c>
-      <c r="K18" s="30">
-        <v>29627.200000000001</v>
-      </c>
-      <c r="L18" s="31">
-        <v>491.046564278326</v>
-      </c>
-      <c r="M18" s="30">
-        <v>-1.1032200000000001</v>
-      </c>
-      <c r="N18" s="31">
-        <v>0.94940379111289996</v>
-      </c>
-      <c r="O18" s="30">
-        <v>-2.1638600000000001</v>
-      </c>
-      <c r="P18" s="31">
-        <v>0.94756156556688498</v>
-      </c>
-      <c r="Q18" s="35" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="7:17" ht="115.5" x14ac:dyDescent="0.25">
-      <c r="G19" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="H19" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="I19" s="30">
-        <v>18366.099999999999</v>
-      </c>
-      <c r="J19" s="31">
-        <v>11195.507941412599</v>
-      </c>
-      <c r="K19" s="30">
-        <v>34292.400000000001</v>
-      </c>
-      <c r="L19" s="31">
-        <v>20525.288342845299</v>
-      </c>
-      <c r="M19" s="30">
-        <v>-1.45282</v>
-      </c>
-      <c r="N19" s="31">
-        <v>-0.49517729383979597</v>
-      </c>
-      <c r="O19" s="30">
-        <v>-2.6620599999999999</v>
-      </c>
-      <c r="P19" s="31">
-        <v>-1.19187764518602</v>
-      </c>
-      <c r="Q19" s="39" t="s">
-        <v>80</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H6:Q6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2398,7 +1897,7 @@
   <dimension ref="A2:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2456,4 +1955,201 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7D4F25-0A5A-44D1-8B8A-CF4A21198441}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection sqref="A1:C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.42578125" style="23" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" style="23" customWidth="1"/>
+    <col min="3" max="3" width="54.42578125" style="23" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>